<commit_message>
add openblas results to graphic
</commit_message>
<xml_diff>
--- a/habr_article/Graphics.xlsx
+++ b/habr_article/Graphics.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vlasov\github\my\mini_gemm\habr_article\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1\gemm project\mini_gemm\habr_article\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBF0B02-F7E4-4FEC-8C90-474163127048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10650" yWindow="4638" windowWidth="19200" windowHeight="11268"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,15 +25,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Запрос — Таблица1" description="Соединение с запросом &quot;Таблица1&quot; в книге." type="5" refreshedVersion="8" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Запрос — Таблица1" description="Соединение с запросом &quot;Таблица1&quot; в книге." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Таблица1;Extended Properties=&quot;&quot;" command="SELECT * FROM [Таблица1]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>function name</t>
   </si>
@@ -75,11 +76,32 @@
   <si>
     <t>AMD Razen 7 5800H</t>
   </si>
+  <si>
+    <t>gemm_v8</t>
+  </si>
+  <si>
+    <t>gemm_openblas</t>
+  </si>
+  <si>
+    <t>frequency (GHz)</t>
+  </si>
+  <si>
+    <t>Max GFLOPS</t>
+  </si>
+  <si>
+    <t>% from maximum</t>
+  </si>
+  <si>
+    <t>GFLOPS openblas</t>
+  </si>
+  <si>
+    <t>Duration openblas (ms)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -217,7 +239,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -254,21 +275,90 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$B$3</c:f>
+              <c:f>Лист1!$F$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> duration (ms)</c:v>
+                  <c:v>Duration openblas (ms)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$F$5:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25.977</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.977</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.977</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.977</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.977</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.977</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.977</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.977</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A496-456F-A0D2-5815D6BEE47F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> duration (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -293,7 +383,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Лист1!$A$4:$A$11</c:f>
+              <c:f>Лист1!$A$5:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -325,33 +415,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$4:$B$11</c:f>
+              <c:f>Лист1!$B$5:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2021</c:v>
+                  <c:v>1991.95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>81</c:v>
+                  <c:v>80.683999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80</c:v>
+                  <c:v>79.063000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35</c:v>
+                  <c:v>35.069000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26</c:v>
+                  <c:v>25.734000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28</c:v>
+                  <c:v>27.471</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27</c:v>
+                  <c:v>26.062000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26</c:v>
+                  <c:v>25.907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -380,21 +470,87 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="3"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$C$3</c:f>
+              <c:f>Лист1!$G$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> GFLOPS</c:v>
+                  <c:v>GFLOPS openblas</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$G$5:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>117.706</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117.706</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>117.706</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>117.706</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>117.706</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>117.706</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>117.706</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>117.706</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-A496-456F-A0D2-5815D6BEE47F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> GFLOPS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -419,7 +575,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Лист1!$A$4:$A$11</c:f>
+              <c:f>Лист1!$A$5:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -451,33 +607,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$C$4:$C$11</c:f>
+              <c:f>Лист1!$C$5:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.51294</c:v>
+                  <c:v>1.5349999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37.748699999999999</c:v>
+                  <c:v>37.896599999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.220599999999997</c:v>
+                  <c:v>38.6736</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>87.361400000000003</c:v>
+                  <c:v>87.189499999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>117.602</c:v>
+                  <c:v>118.81699999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>109.202</c:v>
+                  <c:v>111.30500000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>113.246</c:v>
+                  <c:v>117.322</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>117.602</c:v>
+                  <c:v>118.024</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -523,6 +679,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Этап</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> оптимизации</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -590,6 +806,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Время</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> вычисления, мс</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -638,6 +914,69 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Производительность</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t>, </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>GFLOPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -700,14 +1039,15 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="bg2"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -739,7 +1079,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -747,6 +1086,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -815,30 +1155,82 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="ru-RU"/>
-              <a:t>Перемножение</a:t>
+              <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Перемножение матрицы </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="ru-RU" baseline="0"/>
-              <a:t> матрицы </a:t>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>1152x1152</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>1152x115200</a:t>
+              <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>00 на </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="ru-RU" baseline="0"/>
-              <a:t> на </a:t>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>1152</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>115200x1152</a:t>
+              <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>00</a:t>
             </a:r>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>x1152</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -875,11 +1267,106 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$B$37</c:f>
+              <c:f>Лист1!$F$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duration openblas (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$A$39:$A$45</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>gemm_v1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gemm_v2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gemm_v3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gemm_v4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gemm_v5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>gemm_v6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>gemm_v7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$F$39:$F$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2625.18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2625.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2625.18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2625.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2625.18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2625.18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2625.18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1A15-4D1C-BC8B-7D9F5CCE1423}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$B$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -914,7 +1401,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Лист1!$A$38:$A$44</c:f>
+              <c:f>Лист1!$A$39:$A$45</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -943,30 +1430,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$38:$B$44</c:f>
+              <c:f>Лист1!$B$39:$B$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>22108</c:v>
+                  <c:v>21521.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21708</c:v>
+                  <c:v>20874.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14048</c:v>
+                  <c:v>13555.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3026</c:v>
+                  <c:v>2900.57</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3017</c:v>
+                  <c:v>2879.13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2793</c:v>
+                  <c:v>2650.28</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2697</c:v>
+                  <c:v>2618.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -974,7 +1461,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BC46-4DF6-9DA4-FA638B707056}"/>
+              <c16:uniqueId val="{00000001-1A15-4D1C-BC8B-7D9F5CCE1423}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -988,18 +1475,81 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1319070016"/>
-        <c:axId val="1319069296"/>
+        <c:axId val="505867536"/>
+        <c:axId val="505870776"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="3"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$C$37</c:f>
+              <c:f>Лист1!$G$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GFLOPS openblas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$G$39:$G$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>116.474</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116.474</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>116.474</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>116.474</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>116.474</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>116.474</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>116.474</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1A15-4D1C-BC8B-7D9F5CCE1423}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$C$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1034,28 +1584,31 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Лист1!$A$38:$A$44</c:f>
+              <c:f>Лист1!$A$5:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>gemm_v0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>gemm_v1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>gemm_v2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>gemm_v3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>gemm_v4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>gemm_v5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>gemm_v6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>gemm_v7</c:v>
                 </c:pt>
               </c:strCache>
@@ -1063,30 +1616,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$C$38:$C$44</c:f>
+              <c:f>Лист1!$C$39:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>13.830500000000001</c:v>
+                  <c:v>14.207599999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.0853</c:v>
+                  <c:v>14.647600000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.765699999999999</c:v>
+                  <c:v>22.557200000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>101.04600000000001</c:v>
+                  <c:v>105.41500000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>101.34699999999999</c:v>
+                  <c:v>106.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>109.47499999999999</c:v>
+                  <c:v>115.371</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>113.372</c:v>
+                  <c:v>116.76300000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1094,7 +1647,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-BC46-4DF6-9DA4-FA638B707056}"/>
+              <c16:uniqueId val="{00000003-1A15-4D1C-BC8B-7D9F5CCE1423}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1108,11 +1661,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1312251024"/>
-        <c:axId val="1312257864"/>
+        <c:axId val="1314170384"/>
+        <c:axId val="1314169304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1319070016"/>
+        <c:axId val="505867536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1163,7 +1716,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1230,7 +1782,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1319069296"/>
+        <c:crossAx val="505870776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1239,7 +1791,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1319069296"/>
+        <c:axId val="505870776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1280,17 +1832,16 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="ru-RU"/>
-                  <a:t>Время вычисления</a:t>
+                  <a:t>Время</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="ru-RU" baseline="0"/>
-                  <a:t>, мс</a:t>
+                  <a:t> вычисления, мс</a:t>
                 </a:r>
                 <a:endParaRPr lang="ru-RU"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1357,12 +1908,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1319070016"/>
+        <c:crossAx val="505867536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1312257864"/>
+        <c:axId val="1314169304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1389,7 +1940,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="ru-RU"/>
-                  <a:t>производительность</a:t>
+                  <a:t>Производительность</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="ru-RU" baseline="0"/>
@@ -1399,11 +1950,9 @@
                   <a:rPr lang="en-US" baseline="0"/>
                   <a:t>GFLOPS</a:t>
                 </a:r>
-                <a:endParaRPr lang="ru-RU"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1470,12 +2019,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1312251024"/>
+        <c:crossAx val="1314170384"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="1312251024"/>
+        <c:axId val="1314170384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1485,7 +2034,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1312257864"/>
+        <c:crossAx val="1314169304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1495,14 +2044,15 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="bg2"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1534,7 +2084,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1542,6 +2091,1642 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Производительность</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> на перемножении матриц </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>1152x1152</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> на </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>1152x1152</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> GFLOPS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$A$5:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>gemm_v0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gemm_v1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gemm_v2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gemm_v3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gemm_v4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>gemm_v5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>gemm_v6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>gemm_v7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$C$5:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.5349999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.896599999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38.6736</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>87.189499999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>118.81699999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>111.30500000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>117.322</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>118.024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1221-48E9-88D6-9225589CC47F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="577204280"/>
+        <c:axId val="577202480"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% from maximum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$A$5:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>gemm_v0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gemm_v1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gemm_v2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gemm_v3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gemm_v4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>gemm_v5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>gemm_v6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>gemm_v7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$D$5:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0901988636363635</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.915198863636363</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.467045454545453</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61.924360795454533</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84.387073863636346</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>79.051846590909093</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83.325284090909093</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83.823863636363626</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1221-48E9-88D6-9225589CC47F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="814040216"/>
+        <c:axId val="577202120"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="577204280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Этап</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> оптимизации</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="577202480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="577202480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Производительность</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t>, </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>GFLOPS</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="577204280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="577202120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Процент</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> от теоретического максимума</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="814040216"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="814040216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="577202120"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Производительность</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> на перемножении матриц </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>1152x1152</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>00 на </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>1152</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>00</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>x1152</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$C$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> GFLOPS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$A$39:$A$45</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>gemm_v1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gemm_v2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gemm_v3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gemm_v4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gemm_v5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>gemm_v6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>gemm_v7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$C$39:$C$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>14.207599999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.647600000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.557200000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>105.41500000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>106.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>115.371</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>116.76300000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8B79-4EA3-9D40-8C0E21D5D6EB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="577204280"/>
+        <c:axId val="577202480"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$D$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% from maximum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$A$39:$A$45</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>gemm_v1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gemm_v2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gemm_v3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gemm_v4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>gemm_v5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>gemm_v6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>gemm_v7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$D$39:$D$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10.090624999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.403124999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.020738636363635</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74.868607954545453</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75.42613636363636</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>81.939630681818173</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>82.928267045454547</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8B79-4EA3-9D40-8C0E21D5D6EB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="814040216"/>
+        <c:axId val="577202120"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="577204280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Этап</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> оптимизации</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="577202480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="577202480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Производительность</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t>, </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>GFLOPS</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="577204280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="577202120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Процент</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> от теоретического максимума</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="814040216"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="814040216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="577202120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1656,6 +3841,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2688,20 +4953,1026 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>22224</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>41274</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2728,23 +5999,61 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Диаграмма 2">
+        <xdr:cNvPr id="5" name="Диаграмма 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79208F3B-783D-D99A-5A33-F0EEB0B2B4C4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2972BC2-1B33-4C14-AB89-2F87E375AD3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Диаграмма 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEE16AC7-4D62-6E06-DBEB-F3C67E51437D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2756,7 +6065,45 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>387350</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Диаграмма 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFDBC420-5E2F-4843-9029-710A894E3A3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3061,215 +6408,502 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="A3:C11"/>
+    <sheetView tabSelected="1" topLeftCell="P22" workbookViewId="0">
+      <selection activeCell="AL32" sqref="AL32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" customWidth="1"/>
+    <col min="6" max="6" width="17.08984375" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D1" t="s">
         <v>13</v>
       </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I2">
+        <f>G2*2*2*8</f>
+        <v>140.80000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>2</v>
       </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>2021</v>
-      </c>
-      <c r="C4">
-        <v>1.51294</v>
+      <c r="B5">
+        <v>1991.95</v>
+      </c>
+      <c r="C5">
+        <v>1.5349999999999999</v>
+      </c>
+      <c r="D5">
+        <f>C5/$I$2 * 100</f>
+        <v>1.0901988636363635</v>
+      </c>
+      <c r="F5">
+        <f>$B$14</f>
+        <v>25.977</v>
+      </c>
+      <c r="G5">
+        <f>$C$14</f>
+        <v>117.706</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>81</v>
-      </c>
-      <c r="C5">
-        <v>37.748699999999999</v>
+      <c r="B6">
+        <v>80.683999999999997</v>
+      </c>
+      <c r="C6">
+        <v>37.896599999999999</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D14" si="0">C6/$I$2 * 100</f>
+        <v>26.915198863636363</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F13" si="1">$B$14</f>
+        <v>25.977</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G12" si="2">$C$14</f>
+        <v>117.706</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>80</v>
-      </c>
-      <c r="C6">
-        <v>38.220599999999997</v>
+      <c r="B7">
+        <v>79.063000000000002</v>
+      </c>
+      <c r="C7">
+        <v>38.6736</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>27.467045454545453</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>25.977</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>117.706</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>35</v>
-      </c>
-      <c r="C7">
-        <v>87.361400000000003</v>
+      <c r="B8">
+        <v>35.069000000000003</v>
+      </c>
+      <c r="C8">
+        <v>87.189499999999995</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>61.924360795454533</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>25.977</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>117.706</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>26</v>
-      </c>
-      <c r="C8">
-        <v>117.602</v>
+      <c r="B9">
+        <v>25.734000000000002</v>
+      </c>
+      <c r="C9">
+        <v>118.81699999999999</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>84.387073863636346</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>25.977</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>117.706</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>28</v>
-      </c>
-      <c r="C9">
-        <v>109.202</v>
+      <c r="B10">
+        <v>27.471</v>
+      </c>
+      <c r="C10">
+        <v>111.30500000000001</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>79.051846590909093</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>25.977</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>117.706</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>27</v>
-      </c>
-      <c r="C10">
-        <v>113.246</v>
+      <c r="B11">
+        <v>26.062000000000001</v>
+      </c>
+      <c r="C11">
+        <v>117.322</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>83.325284090909093</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>25.977</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>117.706</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>26</v>
-      </c>
-      <c r="C11">
-        <v>117.602</v>
+      <c r="B12">
+        <v>25.907</v>
+      </c>
+      <c r="C12">
+        <v>118.024</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>83.823863636363626</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>25.977</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>117.706</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>8.0079999999999991</v>
+      </c>
+      <c r="C13">
+        <v>381.82400000000001</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>271.18181818181819</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>25.977</v>
+      </c>
+      <c r="G13">
+        <f>$C$14</f>
+        <v>117.706</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>25.977</v>
+      </c>
+      <c r="C14">
+        <v>117.706</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>83.59801136363636</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>0</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>1</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>2</v>
       </c>
+      <c r="D38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>4</v>
       </c>
-      <c r="B38">
-        <v>22108</v>
-      </c>
-      <c r="C38">
-        <v>13.830500000000001</v>
+      <c r="B39">
+        <v>21521.1</v>
+      </c>
+      <c r="C39">
+        <v>14.207599999999999</v>
+      </c>
+      <c r="D39">
+        <f>C39/$I$2 * 100</f>
+        <v>10.090624999999999</v>
+      </c>
+      <c r="F39">
+        <f>$B$47</f>
+        <v>2625.18</v>
+      </c>
+      <c r="G39">
+        <f>$C$47</f>
+        <v>116.474</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>5</v>
       </c>
-      <c r="B39">
-        <v>21708</v>
-      </c>
-      <c r="C39">
-        <v>14.0853</v>
+      <c r="B40">
+        <v>20874.7</v>
+      </c>
+      <c r="C40">
+        <v>14.647600000000001</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ref="D40:D48" si="3">C40/$I$2 * 100</f>
+        <v>10.403124999999999</v>
+      </c>
+      <c r="F40">
+        <f t="shared" ref="F40:F45" si="4">$B$47</f>
+        <v>2625.18</v>
+      </c>
+      <c r="G40">
+        <f t="shared" ref="G40:G45" si="5">$C$47</f>
+        <v>116.474</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>6</v>
       </c>
-      <c r="B40">
-        <v>14048</v>
-      </c>
-      <c r="C40">
-        <v>21.765699999999999</v>
+      <c r="B41">
+        <v>13555.1</v>
+      </c>
+      <c r="C41">
+        <v>22.557200000000002</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="3"/>
+        <v>16.020738636363635</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="4"/>
+        <v>2625.18</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="5"/>
+        <v>116.474</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>7</v>
       </c>
-      <c r="B41">
-        <v>3026</v>
-      </c>
-      <c r="C41">
-        <v>101.04600000000001</v>
+      <c r="B42">
+        <v>2900.57</v>
+      </c>
+      <c r="C42">
+        <v>105.41500000000001</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="3"/>
+        <v>74.868607954545453</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="4"/>
+        <v>2625.18</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="5"/>
+        <v>116.474</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>8</v>
       </c>
-      <c r="B42">
-        <v>3017</v>
-      </c>
-      <c r="C42">
-        <v>101.34699999999999</v>
+      <c r="B43">
+        <v>2879.13</v>
+      </c>
+      <c r="C43">
+        <v>106.2</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="3"/>
+        <v>75.42613636363636</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="4"/>
+        <v>2625.18</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="5"/>
+        <v>116.474</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>9</v>
       </c>
-      <c r="B43">
-        <v>2793</v>
-      </c>
-      <c r="C43">
-        <v>109.47499999999999</v>
+      <c r="B44">
+        <v>2650.28</v>
+      </c>
+      <c r="C44">
+        <v>115.371</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="3"/>
+        <v>81.939630681818173</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="4"/>
+        <v>2625.18</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="5"/>
+        <v>116.474</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>10</v>
       </c>
-      <c r="B44">
-        <v>2697</v>
-      </c>
-      <c r="C44">
-        <v>113.372</v>
+      <c r="B45">
+        <v>2618.67</v>
+      </c>
+      <c r="C45">
+        <v>116.76300000000001</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="3"/>
+        <v>82.928267045454547</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="4"/>
+        <v>2625.18</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="5"/>
+        <v>116.474</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46">
+        <v>853.97699999999998</v>
+      </c>
+      <c r="C46">
+        <v>358.048</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="3"/>
+        <v>254.29545454545456</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47">
+        <v>2625.18</v>
+      </c>
+      <c r="C47">
+        <v>116.474</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="3"/>
+        <v>82.72301136363636</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add list with parallelism
</commit_message>
<xml_diff>
--- a/habr_article/Graphics.xlsx
+++ b/habr_article/Graphics.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1\gemm project\mini_gemm\habr_article\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBF0B02-F7E4-4FEC-8C90-474163127048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEC1ADE-F799-43B9-80FA-A0CEF9BC10C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="3" r:id="rId1"/>
+    <sheet name="Parallelism" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="29">
   <si>
     <t>function name</t>
   </si>
@@ -97,6 +98,30 @@
   <si>
     <t>Duration openblas (ms)</t>
   </si>
+  <si>
+    <t>#pragma parallel перед циклом по i</t>
+  </si>
+  <si>
+    <t>#pragma parallel перед циклом по k</t>
+  </si>
+  <si>
+    <t>#pragma parallel перед циклом по j</t>
+  </si>
+  <si>
+    <t>number of threads</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> function name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gemm_v8</t>
+  </si>
+  <si>
+    <t>GFLOPS на один поток</t>
+  </si>
+  <si>
+    <t>Тестирование на произведение матриц 1152 x 115200 на 1152 x 115200</t>
+  </si>
 </sst>
 </file>
 
@@ -112,12 +137,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -132,8 +169,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2590,7 +2633,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2850,6 +2893,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="577202120"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3761,6 +3805,1482 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Производительность</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>gemm_v8</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t>, распаллеливание цикла по </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>k c </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t>помощью </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>OpenMP</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v> duration (ms)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="17"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>12</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>14</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>16</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>18</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>20</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>22</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>24</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>26</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>28</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>30</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>32</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="17"/>
+              <c:pt idx="0">
+                <c:v>2631.77</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>1381.09</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>713.05200000000002</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>541.21600000000001</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>475.315</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>461.334</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>442.03500000000003</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>418.952</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>409.05700000000002</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>413.26900000000001</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>410.447</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>415.75700000000001</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>413.87900000000002</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>405.32100000000003</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>407.03</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>409.10199999999998</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>410.46</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5AD5-49B2-8A2E-1248CA64F1F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="734299960"/>
+        <c:axId val="734301400"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v> GFLOPS</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="17"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>12</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>14</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>16</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>18</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>20</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>22</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>24</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>26</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>28</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>30</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>32</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="17"/>
+              <c:pt idx="0">
+                <c:v>116.182</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>221.39400000000001</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>428.81099999999998</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>564.95899999999995</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>643.28899999999999</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>662.78399999999999</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>691.721</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>729.83199999999999</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>747.48699999999997</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>739.86900000000003</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>744.95600000000002</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>735.44100000000003</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>738.77800000000002</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>754.37699999999995</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>751.20899999999995</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>747.40499999999997</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>744.93200000000002</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5AD5-49B2-8A2E-1248CA64F1F9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="738269032"/>
+        <c:axId val="738267232"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="734299960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Количество</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> потоков</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="734301400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="734301400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Время</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> вычисления, мс</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="734299960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="738267232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Производительность, </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>GFLOPS</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="738269032"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="738269032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="738267232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.39844875948655634"/>
+          <c:y val="0.92470041038151307"/>
+          <c:w val="0.21016808570320597"/>
+          <c:h val="4.2533370538505179E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Производительность</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>GFLOPS </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>на один поток</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Parallelism!$K$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GFLOPS на один поток</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Parallelism!$G$6:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Parallelism!$K$6:$K$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>116.182</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>110.697</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>107.20274999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>94.159833333333324</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80.411124999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66.278400000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57.643416666666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>52.130857142857145</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46.717937499999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41.103833333333334</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>37.247799999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33.429136363636367</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30.782416666666666</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29.014499999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26.828892857142854</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24.913499999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>23.279125000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4363-434D-8E53-BDA36AC5DAA5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="739585832"/>
+        <c:axId val="739587272"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="739585832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Количество</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> потоков</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="739587272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="739587272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Производительность</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> на один поток, </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>GFLOPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="739585832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3921,6 +5441,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5457,6 +7057,1012 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6112,6 +8718,85 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2028824</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>79374</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{896CC2CF-5C18-4BC9-93D2-AA747125BB2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>82550</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Диаграмма 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3720541C-2227-2851-9C53-89F656790B0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
@@ -6411,8 +9096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P22" workbookViewId="0">
-      <selection activeCell="AL32" sqref="AL32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6749,7 +9434,7 @@
         <v>14.647600000000001</v>
       </c>
       <c r="D40">
-        <f t="shared" ref="D40:D48" si="3">C40/$I$2 * 100</f>
+        <f t="shared" ref="D40:D47" si="3">C40/$I$2 * 100</f>
         <v>10.403124999999999</v>
       </c>
       <c r="F40">
@@ -6907,6 +9592,694 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A583980-3F2B-4CC9-8981-3D5BC4F38C12}">
+  <dimension ref="A2:P22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="M3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>2642.49</v>
+      </c>
+      <c r="D6">
+        <v>115.711</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6">
+        <v>2631.77</v>
+      </c>
+      <c r="J6">
+        <v>116.182</v>
+      </c>
+      <c r="K6">
+        <f>J6/G6</f>
+        <v>116.182</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6">
+        <v>2610.41</v>
+      </c>
+      <c r="P6">
+        <v>117.133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>1803.02</v>
+      </c>
+      <c r="D7">
+        <v>169.584</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7">
+        <v>1381.09</v>
+      </c>
+      <c r="J7">
+        <v>221.39400000000001</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K7:K22" si="0">J7/G7</f>
+        <v>110.697</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7">
+        <v>2624.09</v>
+      </c>
+      <c r="P7">
+        <v>116.52200000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8">
+        <v>1245.02</v>
+      </c>
+      <c r="D8">
+        <v>245.59</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8">
+        <v>713.05200000000002</v>
+      </c>
+      <c r="J8">
+        <v>428.81099999999998</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>107.20274999999999</v>
+      </c>
+      <c r="M8">
+        <v>4</v>
+      </c>
+      <c r="N8" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8">
+        <v>2645.45</v>
+      </c>
+      <c r="P8">
+        <v>115.581</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>703.43100000000004</v>
+      </c>
+      <c r="D9">
+        <v>434.67599999999999</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9">
+        <v>541.21600000000001</v>
+      </c>
+      <c r="J9">
+        <v>564.95899999999995</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>94.159833333333324</v>
+      </c>
+      <c r="M9">
+        <v>8</v>
+      </c>
+      <c r="N9" t="s">
+        <v>26</v>
+      </c>
+      <c r="O9">
+        <v>2618.65</v>
+      </c>
+      <c r="P9">
+        <v>116.764</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10">
+        <v>728.30700000000002</v>
+      </c>
+      <c r="D10">
+        <v>419.82900000000001</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10">
+        <v>475.315</v>
+      </c>
+      <c r="J10">
+        <v>643.28899999999999</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>80.411124999999998</v>
+      </c>
+      <c r="M10">
+        <v>16</v>
+      </c>
+      <c r="N10" t="s">
+        <v>26</v>
+      </c>
+      <c r="O10">
+        <v>2636.27</v>
+      </c>
+      <c r="P10">
+        <v>115.98399999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>873.77800000000002</v>
+      </c>
+      <c r="D11">
+        <v>349.93400000000003</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11">
+        <v>461.334</v>
+      </c>
+      <c r="J11">
+        <v>662.78399999999999</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>66.278400000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>834.48299999999995</v>
+      </c>
+      <c r="D12">
+        <v>366.41199999999998</v>
+      </c>
+      <c r="G12">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12">
+        <v>442.03500000000003</v>
+      </c>
+      <c r="J12">
+        <v>691.721</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>57.643416666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>838.89</v>
+      </c>
+      <c r="D13">
+        <v>364.48700000000002</v>
+      </c>
+      <c r="G13">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13">
+        <v>418.952</v>
+      </c>
+      <c r="J13">
+        <v>729.83199999999999</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>52.130857142857145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>855.92399999999998</v>
+      </c>
+      <c r="D14">
+        <v>357.23399999999998</v>
+      </c>
+      <c r="G14">
+        <v>16</v>
+      </c>
+      <c r="H14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14">
+        <v>409.05700000000002</v>
+      </c>
+      <c r="J14">
+        <v>747.48699999999997</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>46.717937499999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15">
+        <v>870.54100000000005</v>
+      </c>
+      <c r="D15">
+        <v>351.23500000000001</v>
+      </c>
+      <c r="G15">
+        <v>18</v>
+      </c>
+      <c r="H15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15">
+        <v>413.26900000000001</v>
+      </c>
+      <c r="J15">
+        <v>739.86900000000003</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>41.103833333333334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16">
+        <v>837.08299999999997</v>
+      </c>
+      <c r="D16">
+        <v>365.274</v>
+      </c>
+      <c r="G16">
+        <v>20</v>
+      </c>
+      <c r="H16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16">
+        <v>410.447</v>
+      </c>
+      <c r="J16">
+        <v>744.95600000000002</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>37.247799999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <v>826.56299999999999</v>
+      </c>
+      <c r="D17">
+        <v>369.923</v>
+      </c>
+      <c r="G17">
+        <v>22</v>
+      </c>
+      <c r="H17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17">
+        <v>415.75700000000001</v>
+      </c>
+      <c r="J17">
+        <v>735.44100000000003</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>33.429136363636367</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18">
+        <v>830.95500000000004</v>
+      </c>
+      <c r="D18">
+        <v>367.96800000000002</v>
+      </c>
+      <c r="G18">
+        <v>24</v>
+      </c>
+      <c r="H18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18">
+        <v>413.87900000000002</v>
+      </c>
+      <c r="J18">
+        <v>738.77800000000002</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>30.782416666666666</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19">
+        <v>854.596</v>
+      </c>
+      <c r="D19">
+        <v>357.78899999999999</v>
+      </c>
+      <c r="G19">
+        <v>26</v>
+      </c>
+      <c r="H19" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19">
+        <v>405.32100000000003</v>
+      </c>
+      <c r="J19">
+        <v>754.37699999999995</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>29.014499999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20">
+        <v>858.14700000000005</v>
+      </c>
+      <c r="D20">
+        <v>356.30799999999999</v>
+      </c>
+      <c r="G20">
+        <v>28</v>
+      </c>
+      <c r="H20" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20">
+        <v>407.03</v>
+      </c>
+      <c r="J20">
+        <v>751.20899999999995</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>26.828892857142854</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
+        <v>869.13</v>
+      </c>
+      <c r="D21">
+        <v>351.80599999999998</v>
+      </c>
+      <c r="G21">
+        <v>30</v>
+      </c>
+      <c r="H21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21">
+        <v>409.10199999999998</v>
+      </c>
+      <c r="J21">
+        <v>747.40499999999997</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>24.913499999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22">
+        <v>858.95299999999997</v>
+      </c>
+      <c r="D22">
+        <v>355.97399999999999</v>
+      </c>
+      <c r="G22">
+        <v>32</v>
+      </c>
+      <c r="H22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22">
+        <v>410.46</v>
+      </c>
+      <c r="J22">
+        <v>744.93200000000002</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>23.279125000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="A2:P2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>